<commit_message>
fix bug osd - update pnghk template
</commit_message>
<xml_diff>
--- a/Projects/PNGHK/Data/08_PNGHK_template_2019_05_14.xlsx
+++ b/Projects/PNGHK/Data/08_PNGHK_template_2019_05_14.xlsx
@@ -17,6 +17,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIS!$A$1:$V$105</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIS!$A$1:$V$105</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIS!$A$1:$V$105</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">KPIS!$A$1:$V$105</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -799,14 +800,14 @@
   <dimension ref="A1:AI105"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D86" activeCellId="1" sqref="H53 D86"/>
+      <selection pane="topLeft" activeCell="D86" activeCellId="0" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="78.2959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.3520408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8689,20 +8690,20 @@
   </sheetPr>
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H53" activeCellId="0" sqref="H53"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.1938775510204"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.1989795918367"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.6989795918367"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.515306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="52" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8947,7 +8948,7 @@
         <v>135</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>127</v>

</xml_diff>

<commit_message>
working on 4000 per all categories bug
</commit_message>
<xml_diff>
--- a/Projects/PNGHK/Data/08_PNGHK_template_2019_05_14.xlsx
+++ b/Projects/PNGHK/Data/08_PNGHK_template_2019_05_14.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIS" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,6 +18,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIS!$A$1:$V$105</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIS!$A$1:$V$105</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">KPIS!$A$1:$V$105</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">KPIS!$A$1:$V$105</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -799,15 +800,15 @@
   </sheetPr>
   <dimension ref="A1:AI105"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D86" activeCellId="0" sqref="D86"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A103" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A107" activeCellId="0" sqref="106:107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.3520408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="76.4030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8690,20 +8691,20 @@
   </sheetPr>
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="1" sqref="106:107 F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.515306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.9795918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="52" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>